<commit_message>
adding new test data for creating contact
</commit_message>
<xml_diff>
--- a/src/main/java/com/crm/qa/testdata/FreeCRM_testdata.xlsx
+++ b/src/main/java/com/crm/qa/testdata/FreeCRM_testdata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\E-Banking Automation Mini Project\FreeCRMTest\src\main\java\com\crm\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C43E0CF6-D326-4248-92BF-4EF89ECD08AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57C532F9-752A-474D-A55B-ED52CF31F955}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{DE29F5AA-0372-48E0-A8C5-8053147F7D2F}"/>
   </bookViews>
@@ -47,16 +47,16 @@
     <t>Category</t>
   </si>
   <si>
-    <t>Adidas</t>
-  </si>
-  <si>
     <t>Customer</t>
   </si>
   <si>
-    <t>Abhishek</t>
-  </si>
-  <si>
-    <t>Kumar</t>
+    <t>Reshma</t>
+  </si>
+  <si>
+    <t>Khan</t>
+  </si>
+  <si>
+    <t>Naggaro</t>
   </si>
 </sst>
 </file>
@@ -418,7 +418,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -445,16 +445,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>